<commit_message>
copia de seguridad app
</commit_message>
<xml_diff>
--- a/public/app-gestion-stock.xlsx
+++ b/public/app-gestion-stock.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\app-stock-prioritario\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\app-gestion-stock\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D07D76-C8C2-43F6-BD89-02849E755F07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BBAD077-5100-4C61-A797-4CC578322478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4A431876-5137-4E3B-8F25-94351A4B0413}"/>
   </bookViews>
@@ -31,12 +31,15 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>Inicio de sesion</t>
   </si>
@@ -47,22 +50,10 @@
     <t>Contraseña:</t>
   </si>
   <si>
-    <t>estado_stock</t>
-  </si>
-  <si>
     <t>dif_unid</t>
   </si>
   <si>
-    <t>stock_req</t>
-  </si>
-  <si>
     <t>marca/producto</t>
-  </si>
-  <si>
-    <t>stock_control</t>
-  </si>
-  <si>
-    <t>%_cumplimiento</t>
   </si>
   <si>
     <t>producto1</t>
@@ -98,9 +89,6 @@
     <t>excedido</t>
   </si>
   <si>
-    <t>Accion</t>
-  </si>
-  <si>
     <t>Periodo: muestra informacion solo relacionada con ese periodo, ejemplo: Julio-25. Debe estar relacionado a la fecha actual.</t>
   </si>
   <si>
@@ -111,6 +99,24 @@
   </si>
   <si>
     <t>Filtros: Listas desplegables, deben poder interactuar entre si.</t>
+  </si>
+  <si>
+    <t>stock_require</t>
+  </si>
+  <si>
+    <t>stock_current</t>
+  </si>
+  <si>
+    <t>stock_difference</t>
+  </si>
+  <si>
+    <t>stock_compliance</t>
+  </si>
+  <si>
+    <t>action</t>
+  </si>
+  <si>
+    <t>stock_status</t>
   </si>
 </sst>
 </file>
@@ -615,6 +621,34 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -633,51 +667,23 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -685,7 +691,7 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -727,14 +733,10 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="26" noThreeD="1" sel="0" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp16.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
 </file>
 
@@ -743,7 +745,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="26" noThreeD="1" sel="0" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -759,7 +761,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="26" noThreeD="1" sel="0" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
@@ -846,64 +848,6 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>333375</xdr:colOff>
-          <xdr:row>1</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>3</xdr:col>
-          <xdr:colOff>581025</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2050" name="Drop Down 2" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2050"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002080000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
@@ -1020,64 +964,6 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>560070</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="699550" cy="234080"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="CuadroTexto 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2179320" y="0"/>
-          <a:ext cx="699550" cy="234080"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>Sucursal</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
@@ -2195,13 +2081,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:colOff>142875</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
+      <xdr:colOff>361950</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>209550</xdr:rowOff>
     </xdr:to>
@@ -2218,7 +2104,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10039350" y="2105025"/>
+          <a:off x="10067925" y="2209800"/>
           <a:ext cx="219075" cy="200025"/>
         </a:xfrm>
         <a:prstGeom prst="mathMultiply">
@@ -2261,13 +2147,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:colOff>142875</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
+      <xdr:colOff>361950</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -2284,7 +2170,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10039350" y="2333625"/>
+          <a:off x="10067925" y="2486025"/>
           <a:ext cx="219075" cy="200025"/>
         </a:xfrm>
         <a:prstGeom prst="mathMultiply">
@@ -2327,13 +2213,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:colOff>133350</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
+      <xdr:colOff>352425</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -2350,7 +2236,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10039350" y="2552700"/>
+          <a:off x="10058400" y="2752725"/>
           <a:ext cx="219075" cy="200025"/>
         </a:xfrm>
         <a:prstGeom prst="mathMultiply">
@@ -2393,13 +2279,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:colOff>133350</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
+      <xdr:colOff>352425</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -2416,7 +2302,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10039350" y="2771775"/>
+          <a:off x="10058400" y="3019425"/>
           <a:ext cx="219075" cy="200025"/>
         </a:xfrm>
         <a:prstGeom prst="mathMultiply">
@@ -2459,13 +2345,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:colOff>142875</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
+      <xdr:colOff>361950</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -2482,7 +2368,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10039350" y="2990850"/>
+          <a:off x="10067925" y="3286125"/>
           <a:ext cx="219075" cy="200025"/>
         </a:xfrm>
         <a:prstGeom prst="mathMultiply">
@@ -2525,13 +2411,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:colOff>142875</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
+      <xdr:colOff>361950</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -2548,8 +2434,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10039350" y="3219450"/>
-          <a:ext cx="219075" cy="200025"/>
+          <a:off x="10067925" y="3562350"/>
+          <a:ext cx="219075" cy="190500"/>
         </a:xfrm>
         <a:prstGeom prst="mathMultiply">
           <a:avLst/>
@@ -2591,13 +2477,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
+      <xdr:colOff>152400</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
+      <xdr:colOff>371475</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -2614,7 +2500,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10048875" y="4086225"/>
+          <a:off x="10077450" y="3819525"/>
           <a:ext cx="219075" cy="200025"/>
         </a:xfrm>
         <a:prstGeom prst="mathMultiply">
@@ -2672,7 +2558,7 @@
         <xdr:cNvPr id="34" name="Rectángulo 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BD2A9CA-176A-468D-9FDF-FEFE64BDD54C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000022000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2738,7 +2624,7 @@
         <xdr:cNvPr id="35" name="CuadroTexto 34">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCFBF99D-1FF8-44AE-A9FA-AEA95DB43775}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2812,7 +2698,7 @@
                   <a14:compatExt spid="_x0000_s4097"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1595ED2B-333E-4A04-B9E5-D2700EC8750F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000001100000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2870,7 +2756,7 @@
                   <a14:compatExt spid="_x0000_s4098"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8ADE201-78A7-4672-8DC7-0086112B4FCA}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002100000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2928,7 +2814,7 @@
                   <a14:compatExt spid="_x0000_s4099"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02A6ABFE-1A47-4DF7-8ED6-B9C532781C58}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003100000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2976,7 +2862,7 @@
         <xdr:cNvPr id="5" name="CuadroTexto 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C163C781-33C3-49C9-AA61-11EFA5FD18F3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3034,7 +2920,7 @@
         <xdr:cNvPr id="6" name="CuadroTexto 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51AB4E07-0153-4156-8DA2-E7CAA2ED17DB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3092,7 +2978,7 @@
         <xdr:cNvPr id="7" name="CuadroTexto 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D312AA43-F059-436C-8ACE-B045C4C60D68}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3160,7 +3046,7 @@
                   <a14:compatExt spid="_x0000_s4100"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{266C9975-F006-4FE9-A45E-D05488EFE19B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004100000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3228,7 +3114,7 @@
                   <a14:compatExt spid="_x0000_s4101"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{979E2C6F-F6F3-40A9-A3F3-E54208C18B1F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005100000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3977,7 +3863,7 @@
   <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="T17" sqref="T17"/>
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -3987,7 +3873,7 @@
     <col min="5" max="5" width="6.5" customWidth="1"/>
     <col min="6" max="6" width="10.25" customWidth="1"/>
     <col min="7" max="12" width="11" customWidth="1"/>
-    <col min="13" max="13" width="5.875" customWidth="1"/>
+    <col min="13" max="13" width="6.625" customWidth="1"/>
     <col min="14" max="14" width="8.5" customWidth="1"/>
     <col min="15" max="15" width="5" customWidth="1"/>
   </cols>
@@ -4072,7 +3958,7 @@
       <c r="M5" s="10"/>
       <c r="N5" s="13"/>
       <c r="P5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="19.899999999999999" customHeight="1">
@@ -4091,7 +3977,7 @@
       <c r="M6" s="33"/>
       <c r="N6" s="34"/>
       <c r="P6" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -4110,7 +3996,7 @@
       <c r="M7" s="24"/>
       <c r="N7" s="25"/>
       <c r="P7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -4129,36 +4015,36 @@
       <c r="M8" s="24"/>
       <c r="N8" s="25"/>
       <c r="P8" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="9" customFormat="1" ht="30">
       <c r="A9" s="26"/>
-      <c r="B9" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
+      <c r="B9" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="56"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="56"/>
       <c r="G9" s="41" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="H9" s="41" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="I9" s="41" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="J9" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="K9" s="44" t="s">
-        <v>3</v>
-      </c>
-      <c r="L9" s="44"/>
+        <v>23</v>
+      </c>
+      <c r="K9" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="L9" s="56"/>
       <c r="M9" s="41" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="N9" s="28"/>
       <c r="O9" s="22"/>
@@ -4182,13 +4068,13 @@
     </row>
     <row r="11" spans="1:16" ht="17.45" customHeight="1">
       <c r="A11" s="23"/>
-      <c r="B11" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="47"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="47"/>
+      <c r="B11" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="59"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="59"/>
       <c r="G11" s="38">
         <v>10</v>
       </c>
@@ -4201,10 +4087,10 @@
       <c r="J11" s="39">
         <v>0.5</v>
       </c>
-      <c r="K11" s="45" t="s">
-        <v>10</v>
-      </c>
-      <c r="L11" s="45"/>
+      <c r="K11" s="57" t="s">
+        <v>6</v>
+      </c>
+      <c r="L11" s="57"/>
       <c r="M11" s="38"/>
       <c r="N11" s="25"/>
       <c r="O11" s="2"/>
@@ -4228,13 +4114,13 @@
     </row>
     <row r="13" spans="1:16" ht="17.45" customHeight="1">
       <c r="A13" s="23"/>
-      <c r="B13" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
+      <c r="B13" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="54"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="54"/>
       <c r="G13" s="35">
         <v>15</v>
       </c>
@@ -4247,10 +4133,10 @@
       <c r="J13" s="37">
         <v>0.8</v>
       </c>
-      <c r="K13" s="46" t="s">
-        <v>17</v>
-      </c>
-      <c r="L13" s="46"/>
+      <c r="K13" s="58" t="s">
+        <v>13</v>
+      </c>
+      <c r="L13" s="58"/>
       <c r="M13" s="35"/>
       <c r="N13" s="25"/>
       <c r="O13" s="2"/>
@@ -4274,13 +4160,13 @@
     </row>
     <row r="15" spans="1:16" ht="17.45" customHeight="1">
       <c r="A15" s="23"/>
-      <c r="B15" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
+      <c r="B15" s="54" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="54"/>
       <c r="G15" s="35">
         <v>15</v>
       </c>
@@ -4293,10 +4179,10 @@
       <c r="J15" s="37">
         <v>1.1333333333333333</v>
       </c>
-      <c r="K15" s="46" t="s">
-        <v>19</v>
-      </c>
-      <c r="L15" s="46"/>
+      <c r="K15" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="L15" s="58"/>
       <c r="M15" s="35"/>
       <c r="N15" s="25"/>
       <c r="O15" s="2"/>
@@ -4320,13 +4206,13 @@
     </row>
     <row r="17" spans="1:15" ht="17.45" customHeight="1">
       <c r="A17" s="23"/>
-      <c r="B17" s="42" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
+      <c r="B17" s="54" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="54"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="54"/>
       <c r="G17" s="35">
         <v>20</v>
       </c>
@@ -4339,10 +4225,10 @@
       <c r="J17" s="37">
         <v>0.9</v>
       </c>
-      <c r="K17" s="46" t="s">
-        <v>17</v>
-      </c>
-      <c r="L17" s="46"/>
+      <c r="K17" s="58" t="s">
+        <v>13</v>
+      </c>
+      <c r="L17" s="58"/>
       <c r="M17" s="35"/>
       <c r="N17" s="25"/>
       <c r="O17" s="2"/>
@@ -4366,13 +4252,13 @@
     </row>
     <row r="19" spans="1:15" ht="17.45" customHeight="1">
       <c r="A19" s="23"/>
-      <c r="B19" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
+      <c r="B19" s="54" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="54"/>
       <c r="G19" s="35">
         <v>25</v>
       </c>
@@ -4385,10 +4271,10 @@
       <c r="J19" s="37">
         <v>0.6</v>
       </c>
-      <c r="K19" s="46" t="s">
-        <v>10</v>
-      </c>
-      <c r="L19" s="46"/>
+      <c r="K19" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="L19" s="58"/>
       <c r="M19" s="35"/>
       <c r="N19" s="25"/>
       <c r="O19" s="2"/>
@@ -4412,13 +4298,13 @@
     </row>
     <row r="21" spans="1:15" ht="17.45" customHeight="1">
       <c r="A21" s="23"/>
-      <c r="B21" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="42"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42"/>
+      <c r="B21" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="54"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="54"/>
       <c r="G21" s="35">
         <v>30</v>
       </c>
@@ -4431,10 +4317,10 @@
       <c r="J21" s="37">
         <v>0.9</v>
       </c>
-      <c r="K21" s="46" t="s">
-        <v>17</v>
-      </c>
-      <c r="L21" s="46"/>
+      <c r="K21" s="58" t="s">
+        <v>13</v>
+      </c>
+      <c r="L21" s="58"/>
       <c r="M21" s="35"/>
       <c r="N21" s="25"/>
       <c r="O21" s="2"/>
@@ -4458,13 +4344,13 @@
     </row>
     <row r="23" spans="1:15" ht="17.45" customHeight="1">
       <c r="A23" s="23"/>
-      <c r="B23" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" s="43"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="43"/>
+      <c r="B23" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="55"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="55"/>
+      <c r="F23" s="55"/>
       <c r="G23" s="36">
         <v>8</v>
       </c>
@@ -4477,10 +4363,10 @@
       <c r="J23" s="37">
         <v>1.5</v>
       </c>
-      <c r="K23" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="L23" s="46"/>
+      <c r="K23" s="58" t="s">
+        <v>14</v>
+      </c>
+      <c r="L23" s="58"/>
       <c r="M23" s="36"/>
       <c r="N23" s="25"/>
       <c r="O23" s="2"/>
@@ -4650,29 +4536,7 @@
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2050" r:id="rId4" name="Drop Down 2">
-              <controlPr defaultSize="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>2</xdr:col>
-                    <xdr:colOff>333375</xdr:colOff>
-                    <xdr:row>1</xdr:row>
-                    <xdr:rowOff>57150</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>3</xdr:col>
-                    <xdr:colOff>581025</xdr:colOff>
-                    <xdr:row>2</xdr:row>
-                    <xdr:rowOff>57150</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="2054" r:id="rId5" name="Drop Down 6">
+            <control shapeId="2054" r:id="rId4" name="Drop Down 6">
               <controlPr defaultSize="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4694,7 +4558,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2055" r:id="rId6" name="Drop Down 7">
+            <control shapeId="2055" r:id="rId5" name="Drop Down 7">
               <controlPr defaultSize="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4716,7 +4580,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2056" r:id="rId7" name="Button 8">
+            <control shapeId="2056" r:id="rId6" name="Button 8">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
@@ -4738,7 +4602,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2057" r:id="rId8" name="Button 9">
+            <control shapeId="2057" r:id="rId7" name="Button 9">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
@@ -4760,7 +4624,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2058" r:id="rId9" name="Button 10">
+            <control shapeId="2058" r:id="rId8" name="Button 10">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
@@ -4782,7 +4646,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2059" r:id="rId10" name="Button 11">
+            <control shapeId="2059" r:id="rId9" name="Button 11">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
@@ -4804,7 +4668,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2060" r:id="rId11" name="Drop Down 12">
+            <control shapeId="2060" r:id="rId10" name="Drop Down 12">
               <controlPr defaultSize="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4826,7 +4690,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2061" r:id="rId12" name="Drop Down 13">
+            <control shapeId="2061" r:id="rId11" name="Drop Down 13">
               <controlPr defaultSize="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4848,7 +4712,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2062" r:id="rId13" name="Drop Down 14">
+            <control shapeId="2062" r:id="rId12" name="Drop Down 14">
               <controlPr defaultSize="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4870,7 +4734,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2063" r:id="rId14" name="Drop Down 15">
+            <control shapeId="2063" r:id="rId13" name="Drop Down 15">
               <controlPr defaultSize="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4949,48 +4813,48 @@
       <c r="N2" s="5"/>
     </row>
     <row r="3" spans="1:15" ht="18" customHeight="1">
-      <c r="A3" s="50"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
+      <c r="A3" s="44"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
     </row>
     <row r="4" spans="1:15" s="20" customFormat="1" ht="23.45" customHeight="1">
-      <c r="A4" s="48"/>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="49"/>
-      <c r="L4" s="49"/>
-      <c r="M4" s="49"/>
-      <c r="N4" s="51"/>
+      <c r="A4" s="42"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="43"/>
+      <c r="N4" s="45"/>
     </row>
     <row r="5" spans="1:15" ht="29.25" customHeight="1">
       <c r="A5" s="8"/>
-      <c r="B5" s="55" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="63" t="s">
+      <c r="B5" s="64" t="s">
         <v>4</v>
+      </c>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="51" t="s">
+        <v>3</v>
       </c>
       <c r="H5" s="40"/>
       <c r="I5" s="66"/>
@@ -5019,18 +4883,18 @@
     <row r="7" spans="1:15">
       <c r="A7" s="8"/>
       <c r="B7" s="67" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="61"/>
-      <c r="G7" s="64">
         <v>5</v>
       </c>
-      <c r="H7" s="58"/>
-      <c r="I7" s="59"/>
-      <c r="J7" s="59"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="52">
+        <v>5</v>
+      </c>
+      <c r="H7" s="49"/>
+      <c r="I7" s="61"/>
+      <c r="J7" s="61"/>
       <c r="K7" s="24"/>
       <c r="L7" s="24"/>
       <c r="M7" s="24"/>
@@ -5053,20 +4917,20 @@
       <c r="N8" s="24"/>
     </row>
     <row r="9" spans="1:15" s="9" customFormat="1" ht="15">
-      <c r="A9" s="60"/>
-      <c r="B9" s="68" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="62"/>
-      <c r="G9" s="65">
+      <c r="A9" s="50"/>
+      <c r="B9" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="58"/>
-      <c r="I9" s="59"/>
-      <c r="J9" s="59"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="53">
+        <v>10</v>
+      </c>
+      <c r="H9" s="49"/>
+      <c r="I9" s="61"/>
+      <c r="J9" s="61"/>
       <c r="K9" s="40"/>
       <c r="L9" s="27"/>
       <c r="M9" s="27"/>
@@ -5076,14 +4940,14 @@
       <c r="A10" s="27"/>
       <c r="B10" s="27"/>
       <c r="C10" s="27"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="60"/>
-      <c r="F10" s="60"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="60"/>
-      <c r="J10" s="60"/>
-      <c r="K10" s="60"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="50"/>
+      <c r="I10" s="50"/>
+      <c r="J10" s="50"/>
+      <c r="K10" s="50"/>
       <c r="L10" s="40"/>
       <c r="M10" s="27"/>
       <c r="N10" s="27"/>
@@ -5101,7 +4965,7 @@
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
-      <c r="M11" s="57"/>
+      <c r="M11" s="48"/>
       <c r="N11" s="24"/>
       <c r="O11" s="2"/>
     </row>
@@ -5135,8 +4999,8 @@
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
-      <c r="M13" s="57"/>
-      <c r="N13" s="52"/>
+      <c r="M13" s="48"/>
+      <c r="N13" s="46"/>
       <c r="O13" s="2"/>
     </row>
     <row r="14" spans="1:15" ht="3.75" customHeight="1">
@@ -5153,24 +5017,24 @@
       <c r="K14" s="40"/>
       <c r="L14" s="40"/>
       <c r="M14" s="40"/>
-      <c r="N14" s="53"/>
+      <c r="N14" s="47"/>
       <c r="O14" s="2"/>
     </row>
     <row r="15" spans="1:15" ht="17.45" customHeight="1">
       <c r="A15" s="23"/>
-      <c r="B15" s="56"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="57"/>
-      <c r="H15" s="57"/>
-      <c r="I15" s="57"/>
-      <c r="J15" s="58"/>
-      <c r="K15" s="59"/>
-      <c r="L15" s="59"/>
-      <c r="M15" s="57"/>
-      <c r="N15" s="52"/>
+      <c r="B15" s="60"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="48"/>
+      <c r="J15" s="49"/>
+      <c r="K15" s="61"/>
+      <c r="L15" s="61"/>
+      <c r="M15" s="48"/>
+      <c r="N15" s="46"/>
       <c r="O15" s="2"/>
     </row>
     <row r="16" spans="1:15" ht="3.75" customHeight="1">
@@ -5187,24 +5051,24 @@
       <c r="K16" s="40"/>
       <c r="L16" s="40"/>
       <c r="M16" s="40"/>
-      <c r="N16" s="53"/>
+      <c r="N16" s="47"/>
       <c r="O16" s="2"/>
     </row>
     <row r="17" spans="1:15" ht="17.45" customHeight="1">
       <c r="A17" s="23"/>
-      <c r="B17" s="56"/>
-      <c r="C17" s="56"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="56"/>
-      <c r="F17" s="56"/>
-      <c r="G17" s="57"/>
-      <c r="H17" s="57"/>
-      <c r="I17" s="57"/>
-      <c r="J17" s="58"/>
-      <c r="K17" s="59"/>
-      <c r="L17" s="59"/>
-      <c r="M17" s="57"/>
-      <c r="N17" s="52"/>
+      <c r="B17" s="60"/>
+      <c r="C17" s="60"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="60"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="49"/>
+      <c r="K17" s="61"/>
+      <c r="L17" s="61"/>
+      <c r="M17" s="48"/>
+      <c r="N17" s="46"/>
       <c r="O17" s="2"/>
     </row>
     <row r="18" spans="1:15" ht="3.75" customHeight="1">
@@ -5221,7 +5085,7 @@
       <c r="K18" s="40"/>
       <c r="L18" s="40"/>
       <c r="M18" s="40"/>
-      <c r="N18" s="53"/>
+      <c r="N18" s="47"/>
       <c r="O18" s="2"/>
     </row>
     <row r="19" spans="1:15" ht="17.45" customHeight="1">
@@ -5237,8 +5101,8 @@
       <c r="J19" s="8"/>
       <c r="K19" s="8"/>
       <c r="L19" s="8"/>
-      <c r="M19" s="57"/>
-      <c r="N19" s="52"/>
+      <c r="M19" s="48"/>
+      <c r="N19" s="46"/>
       <c r="O19" s="2"/>
     </row>
     <row r="20" spans="1:15" ht="3.75" customHeight="1">
@@ -5255,7 +5119,7 @@
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
       <c r="M20" s="40"/>
-      <c r="N20" s="53"/>
+      <c r="N20" s="47"/>
       <c r="O20" s="2"/>
     </row>
     <row r="21" spans="1:15" ht="17.45" customHeight="1">
@@ -5271,8 +5135,8 @@
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
       <c r="L21" s="8"/>
-      <c r="M21" s="57"/>
-      <c r="N21" s="52"/>
+      <c r="M21" s="48"/>
+      <c r="N21" s="46"/>
       <c r="O21" s="2"/>
     </row>
     <row r="22" spans="1:15" ht="3.75" customHeight="1">
@@ -5289,7 +5153,7 @@
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
       <c r="M22" s="40"/>
-      <c r="N22" s="53"/>
+      <c r="N22" s="47"/>
       <c r="O22" s="2"/>
     </row>
     <row r="23" spans="1:15" ht="17.45" customHeight="1">
@@ -5305,8 +5169,8 @@
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
-      <c r="M23" s="57"/>
-      <c r="N23" s="52"/>
+      <c r="M23" s="48"/>
+      <c r="N23" s="46"/>
       <c r="O23" s="2"/>
     </row>
     <row r="24" spans="1:15" ht="17.45" customHeight="1">
@@ -5323,7 +5187,7 @@
       <c r="K24" s="24"/>
       <c r="L24" s="24"/>
       <c r="M24" s="24"/>
-      <c r="N24" s="52"/>
+      <c r="N24" s="46"/>
       <c r="O24" s="2"/>
     </row>
     <row r="25" spans="1:15" ht="17.45" customHeight="1">
@@ -5340,7 +5204,7 @@
       <c r="K25" s="24"/>
       <c r="L25" s="24"/>
       <c r="M25" s="24"/>
-      <c r="N25" s="52"/>
+      <c r="N25" s="46"/>
       <c r="O25" s="2"/>
     </row>
     <row r="26" spans="1:15" ht="17.45" customHeight="1">
@@ -5357,7 +5221,7 @@
       <c r="K26" s="24"/>
       <c r="L26" s="24"/>
       <c r="M26" s="24"/>
-      <c r="N26" s="52"/>
+      <c r="N26" s="46"/>
       <c r="O26" s="2"/>
     </row>
     <row r="27" spans="1:15" ht="17.45" customHeight="1">
@@ -5374,7 +5238,7 @@
       <c r="K27" s="24"/>
       <c r="L27" s="24"/>
       <c r="M27" s="24"/>
-      <c r="N27" s="52"/>
+      <c r="N27" s="46"/>
       <c r="O27" s="2"/>
     </row>
     <row r="28" spans="1:15" ht="17.45" customHeight="1">
@@ -5391,7 +5255,7 @@
       <c r="K28" s="24"/>
       <c r="L28" s="24"/>
       <c r="M28" s="24"/>
-      <c r="N28" s="52"/>
+      <c r="N28" s="46"/>
       <c r="O28" s="2"/>
     </row>
     <row r="29" spans="1:15" ht="17.45" customHeight="1">
@@ -5408,7 +5272,7 @@
       <c r="K29" s="24"/>
       <c r="L29" s="24"/>
       <c r="M29" s="24"/>
-      <c r="N29" s="52"/>
+      <c r="N29" s="46"/>
       <c r="O29" s="2"/>
     </row>
     <row r="30" spans="1:15" ht="17.45" customHeight="1">
@@ -5447,16 +5311,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="I7:J7"/>
     <mergeCell ref="B15:F15"/>
     <mergeCell ref="K15:L15"/>
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="K17:L17"/>
     <mergeCell ref="B9:F9"/>
     <mergeCell ref="I9:J9"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="I7:J7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="271" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>